<commit_message>
update TD2 and TG3
</commit_message>
<xml_diff>
--- a/MiddleAssignment_LeTuanSang/MiddleAssignment_TestDesign2/TestDesign2_LeTuanSang_updated.xlsx
+++ b/MiddleAssignment_LeTuanSang/MiddleAssignment_TestDesign2/TestDesign2_LeTuanSang_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NashTechHomeWork_LeTuanSang\MiddleAssignment_LeTuanSang\MiddleAssignment_TestDesign2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660C4AC8-3918-43A4-857E-DAF0EC369FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59518B44-A8E4-4800-A66E-4B6BA7F8F929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6717,8 +6717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AMJ229"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>